<commit_message>
Added code to make the excel parts work when the sheet is empty
</commit_message>
<xml_diff>
--- a/Master.xlsx
+++ b/Master.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasg17/Documents/GitHub/Health-Innovation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13D0F59-4A96-DC47-9EDD-7AE94A122EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4088CA1F-B4E7-304C-A052-CEF21BD7FA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{7B871D28-6C56-6A4C-8DC7-F3E0A8269B8A}"/>
   </bookViews>
   <sheets>
-    <sheet name="SV Health" sheetId="1" r:id="rId1"/>
+    <sheet name="SV Health Investors, LLC" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -113,17 +113,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,9 +142,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0ED0BE-763C-6D4C-8358-322C45E67976}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P26" sqref="P26"/>
@@ -474,185 +466,180 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>229</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2">
         <v>510142</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>510142</v>
       </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1"/>
+      <c r="K2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>532</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>311490</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>311490</v>
       </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1"/>
+      <c r="K3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>88786108</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>21098</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <v>907032</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>907032</v>
       </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1"/>
+      <c r="K4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>10420</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <v>1488596</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <v>1488596</v>
       </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1"/>
+      <c r="K5">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added years and worked on issue with dropdown
</commit_message>
<xml_diff>
--- a/Master.xlsx
+++ b/Master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasg17/Documents/GitHub/Health-Innovation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4088CA1F-B4E7-304C-A052-CEF21BD7FA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E214E434-E1E6-0449-81A7-7DC8342E7A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{7B871D28-6C56-6A4C-8DC7-F3E0A8269B8A}"/>
   </bookViews>
@@ -35,7 +35,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
+  <si>
+    <t>Year</t>
+  </si>
   <si>
     <t>nameOfIssuer</t>
   </si>
@@ -162,9 +165,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -202,7 +205,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -308,7 +311,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -450,7 +453,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -458,15 +461,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0ED0BE-763C-6D4C-8358-322C45E67976}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,10 +503,13 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2000</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -511,14 +517,14 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
         <v>229</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>510142</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
@@ -526,19 +532,22 @@
       <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="I2">
-        <v>0</v>
+      <c r="I2" t="s">
+        <v>17</v>
       </c>
       <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
         <v>510142</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2000</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -546,14 +555,14 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3">
         <v>532</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>311490</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
       </c>
       <c r="G3" t="s">
         <v>15</v>
@@ -561,34 +570,37 @@
       <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="I3">
-        <v>0</v>
+      <c r="I3" t="s">
+        <v>17</v>
       </c>
       <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>311490</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>20</v>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2000</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
         <v>88786108</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>21098</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>907032</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
@@ -596,34 +608,37 @@
       <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="I4">
-        <v>0</v>
+      <c r="I4" t="s">
+        <v>17</v>
       </c>
       <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
         <v>907032</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>22</v>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2000</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5">
         <v>10420</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1488596</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
       </c>
       <c r="G5" t="s">
         <v>15</v>
@@ -631,13 +646,168 @@
       <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="I5">
-        <v>0</v>
+      <c r="I5" t="s">
+        <v>17</v>
       </c>
       <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <v>1488596</v>
       </c>
-      <c r="K5">
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2022</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>229</v>
+      </c>
+      <c r="F6">
+        <v>510142</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>510142</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2022</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>532</v>
+      </c>
+      <c r="F7">
+        <v>311490</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>311490</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2022</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>88786108</v>
+      </c>
+      <c r="E8">
+        <v>21098</v>
+      </c>
+      <c r="F8">
+        <v>907032</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>907032</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2022</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9">
+        <v>10420</v>
+      </c>
+      <c r="F9">
+        <v>1488596</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1488596</v>
+      </c>
+      <c r="L9">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed the file to a method and created the test file to run it
</commit_message>
<xml_diff>
--- a/Master.xlsx
+++ b/Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasg17/Documents/GitHub/Health-Innovation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F63286C3-A18A-A044-801E-A3C46EB462BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{57EBFEF9-D711-1C42-9B3C-83FC91E462F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="760" windowWidth="28060" windowHeight="17440" xr2:uid="{7B871D28-6C56-6A4C-8DC7-F3E0A8269B8A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11506" uniqueCount="867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11879" uniqueCount="867">
   <si>
     <t>COM NEW</t>
   </si>
@@ -2989,7 +2989,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DBE7DD-EA50-0848-ABCD-4874656132C1}">
-  <dimension ref="A1:L2115"/>
+  <dimension ref="A1:L2181"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0"/>
   </sheetViews>
@@ -77779,7 +77779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2113" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2113">
         <v>2013</v>
       </c>
@@ -77814,7 +77814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2114" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2114">
         <v>2013</v>
       </c>
@@ -77849,7 +77849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2115">
         <v>2013</v>
       </c>
@@ -77881,6 +77881,2514 @@
         <v>0</v>
       </c>
       <c r="K2115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2116" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2116">
+        <v>2023</v>
+      </c>
+      <c r="B2116" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2116" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2116" s="1">
+        <v>3.5104000000000003E+104</v>
+      </c>
+      <c r="E2116" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2116">
+        <v>52997676</v>
+      </c>
+      <c r="G2116">
+        <v>4163211</v>
+      </c>
+      <c r="H2116" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2116" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2116">
+        <v>4163211</v>
+      </c>
+      <c r="K2116">
+        <v>0</v>
+      </c>
+      <c r="L2116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2117" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2117">
+        <v>2023</v>
+      </c>
+      <c r="B2117" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2117" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2117">
+        <v>282559103</v>
+      </c>
+      <c r="E2117" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2117">
+        <v>176277677</v>
+      </c>
+      <c r="G2117">
+        <v>11416948</v>
+      </c>
+      <c r="H2117" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2117" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2117">
+        <v>11416948</v>
+      </c>
+      <c r="K2117">
+        <v>0</v>
+      </c>
+      <c r="L2117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2118" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2118">
+        <v>2023</v>
+      </c>
+      <c r="B2118" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2118" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2118" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2118" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2118">
+        <v>30129403</v>
+      </c>
+      <c r="G2118">
+        <v>4398453</v>
+      </c>
+      <c r="H2118" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2118" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2118">
+        <v>4398453</v>
+      </c>
+      <c r="K2118">
+        <v>0</v>
+      </c>
+      <c r="L2118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2119" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2119">
+        <v>2023</v>
+      </c>
+      <c r="B2119" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2119" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2119">
+        <v>4890109</v>
+      </c>
+      <c r="E2119" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2119">
+        <v>45988456</v>
+      </c>
+      <c r="G2119">
+        <v>4810508</v>
+      </c>
+      <c r="H2119" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2119" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2119">
+        <v>4810508</v>
+      </c>
+      <c r="K2119">
+        <v>0</v>
+      </c>
+      <c r="L2119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2120" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2120">
+        <v>2023</v>
+      </c>
+      <c r="B2120" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2120" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2120" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2120" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2120">
+        <v>61968061</v>
+      </c>
+      <c r="G2120">
+        <v>14932063</v>
+      </c>
+      <c r="H2120" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2120" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2120">
+        <v>14932063</v>
+      </c>
+      <c r="K2120">
+        <v>0</v>
+      </c>
+      <c r="L2120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2121" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2121">
+        <v>2023</v>
+      </c>
+      <c r="B2121" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2121" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2121">
+        <v>8064107</v>
+      </c>
+      <c r="E2121" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2121">
+        <v>112142236</v>
+      </c>
+      <c r="G2121">
+        <v>8263982</v>
+      </c>
+      <c r="H2121" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2121" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2121">
+        <v>8263982</v>
+      </c>
+      <c r="K2121">
+        <v>0</v>
+      </c>
+      <c r="L2121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2122" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2122">
+        <v>2023</v>
+      </c>
+      <c r="B2122" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2122" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2122" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2122" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2122">
+        <v>53713988</v>
+      </c>
+      <c r="G2122">
+        <v>4691178</v>
+      </c>
+      <c r="H2122" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2122" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2122">
+        <v>4691178</v>
+      </c>
+      <c r="K2122">
+        <v>0</v>
+      </c>
+      <c r="L2122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2123" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2123">
+        <v>2023</v>
+      </c>
+      <c r="B2123" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2123" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2123">
+        <v>37326105</v>
+      </c>
+      <c r="E2123" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2123">
+        <v>89264824</v>
+      </c>
+      <c r="G2123">
+        <v>5551295</v>
+      </c>
+      <c r="H2123" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2123" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2123">
+        <v>5551295</v>
+      </c>
+      <c r="K2123">
+        <v>0</v>
+      </c>
+      <c r="L2123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2124" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2124">
+        <v>2023</v>
+      </c>
+      <c r="B2124" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2124" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2124" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2124" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2124">
+        <v>35757583</v>
+      </c>
+      <c r="G2124">
+        <v>9459678</v>
+      </c>
+      <c r="H2124" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2124" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2124">
+        <v>9459678</v>
+      </c>
+      <c r="K2124">
+        <v>0</v>
+      </c>
+      <c r="L2124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2125" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2125">
+        <v>2023</v>
+      </c>
+      <c r="B2125" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2125" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2125" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2125" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2125">
+        <v>1003779130</v>
+      </c>
+      <c r="G2125">
+        <v>10719555</v>
+      </c>
+      <c r="H2125" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2125" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2125">
+        <v>10719555</v>
+      </c>
+      <c r="K2125">
+        <v>0</v>
+      </c>
+      <c r="L2125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2126" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2126">
+        <v>2023</v>
+      </c>
+      <c r="B2126" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2126" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2126" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2126" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2126">
+        <v>40940447</v>
+      </c>
+      <c r="G2126">
+        <v>6416998</v>
+      </c>
+      <c r="H2126" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2126" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2126">
+        <v>6416998</v>
+      </c>
+      <c r="K2126">
+        <v>0</v>
+      </c>
+      <c r="L2126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2127" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2127">
+        <v>2023</v>
+      </c>
+      <c r="B2127" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2127" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2127" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2127" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2127">
+        <v>69890000</v>
+      </c>
+      <c r="G2127">
+        <v>1000000</v>
+      </c>
+      <c r="H2127" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2127" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2127">
+        <v>1000000</v>
+      </c>
+      <c r="K2127">
+        <v>0</v>
+      </c>
+      <c r="L2127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2128" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2128">
+        <v>2023</v>
+      </c>
+      <c r="B2128" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2128" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2128">
+        <v>88786108</v>
+      </c>
+      <c r="E2128" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2128">
+        <v>16072000</v>
+      </c>
+      <c r="G2128">
+        <v>800000</v>
+      </c>
+      <c r="H2128" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2128" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2128">
+        <v>800000</v>
+      </c>
+      <c r="K2128">
+        <v>0</v>
+      </c>
+      <c r="L2128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2129" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2129">
+        <v>2023</v>
+      </c>
+      <c r="B2129" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2129" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2129" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2129" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2129">
+        <v>136958573</v>
+      </c>
+      <c r="G2129">
+        <v>532892</v>
+      </c>
+      <c r="H2129" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2129" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2129">
+        <v>532892</v>
+      </c>
+      <c r="K2129">
+        <v>0</v>
+      </c>
+      <c r="L2129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2130" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2130">
+        <v>2023</v>
+      </c>
+      <c r="B2130" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2130" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2130" s="1">
+        <v>9.2029999999999997E+108</v>
+      </c>
+      <c r="E2130" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2130">
+        <v>10118914</v>
+      </c>
+      <c r="G2130">
+        <v>3525754</v>
+      </c>
+      <c r="H2130" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2130" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2130">
+        <v>3525754</v>
+      </c>
+      <c r="K2130">
+        <v>0</v>
+      </c>
+      <c r="L2130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2131" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2131">
+        <v>2023</v>
+      </c>
+      <c r="B2131" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2131" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2131" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2131" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2131">
+        <v>12796009</v>
+      </c>
+      <c r="G2131">
+        <v>1400001</v>
+      </c>
+      <c r="H2131" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2131" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2131">
+        <v>1400001</v>
+      </c>
+      <c r="K2131">
+        <v>0</v>
+      </c>
+      <c r="L2131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2132" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2132">
+        <v>2023</v>
+      </c>
+      <c r="B2132" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2132" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2132" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2132" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2132">
+        <v>6240259</v>
+      </c>
+      <c r="G2132">
+        <v>6501624</v>
+      </c>
+      <c r="H2132" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2132" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2132">
+        <v>6501624</v>
+      </c>
+      <c r="K2132">
+        <v>0</v>
+      </c>
+      <c r="L2132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2133" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2133">
+        <v>2023</v>
+      </c>
+      <c r="B2133" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2133" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2133" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2133" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2133">
+        <v>62557433</v>
+      </c>
+      <c r="G2133">
+        <v>6416147</v>
+      </c>
+      <c r="H2133" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2133" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2133">
+        <v>6416147</v>
+      </c>
+      <c r="K2133">
+        <v>0</v>
+      </c>
+      <c r="L2133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2134" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2134">
+        <v>2023</v>
+      </c>
+      <c r="B2134" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2134" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2134">
+        <v>207523101</v>
+      </c>
+      <c r="E2134" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2134">
+        <v>5725631</v>
+      </c>
+      <c r="G2134">
+        <v>6991003</v>
+      </c>
+      <c r="H2134" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2134" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2134">
+        <v>6991003</v>
+      </c>
+      <c r="K2134">
+        <v>0</v>
+      </c>
+      <c r="L2134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2135" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2135">
+        <v>2023</v>
+      </c>
+      <c r="B2135" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2135" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2135" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2135" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2135">
+        <v>9516400</v>
+      </c>
+      <c r="G2135">
+        <v>1286000</v>
+      </c>
+      <c r="H2135" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2135" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2135">
+        <v>1286000</v>
+      </c>
+      <c r="K2135">
+        <v>0</v>
+      </c>
+      <c r="L2135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2136" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2136">
+        <v>2023</v>
+      </c>
+      <c r="B2136" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2136" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2136" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2136" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2136">
+        <v>72427670</v>
+      </c>
+      <c r="G2136">
+        <v>10604344</v>
+      </c>
+      <c r="H2136" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2136" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2136">
+        <v>10604344</v>
+      </c>
+      <c r="K2136">
+        <v>0</v>
+      </c>
+      <c r="L2136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2137" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2137">
+        <v>2023</v>
+      </c>
+      <c r="B2137" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2137" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2137" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2137" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2137">
+        <v>103475400</v>
+      </c>
+      <c r="G2137">
+        <v>6940000</v>
+      </c>
+      <c r="H2137" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2137" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2137">
+        <v>6940000</v>
+      </c>
+      <c r="K2137">
+        <v>0</v>
+      </c>
+      <c r="L2137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2138" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2138">
+        <v>2023</v>
+      </c>
+      <c r="B2138" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2138" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2138" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2138" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2138">
+        <v>95826884</v>
+      </c>
+      <c r="G2138">
+        <v>7809852</v>
+      </c>
+      <c r="H2138" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2138" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2138">
+        <v>7809852</v>
+      </c>
+      <c r="K2138">
+        <v>0</v>
+      </c>
+      <c r="L2138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2139" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2139">
+        <v>2023</v>
+      </c>
+      <c r="B2139" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2139" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2139" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2139" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2139">
+        <v>34586733</v>
+      </c>
+      <c r="G2139">
+        <v>13150849</v>
+      </c>
+      <c r="H2139" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2139" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2139">
+        <v>13150849</v>
+      </c>
+      <c r="K2139">
+        <v>0</v>
+      </c>
+      <c r="L2139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2140" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2140">
+        <v>2023</v>
+      </c>
+      <c r="B2140" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2140" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2140" s="1">
+        <v>2.9336999999999999E+106</v>
+      </c>
+      <c r="E2140" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2140">
+        <v>28992872</v>
+      </c>
+      <c r="G2140">
+        <v>2122465</v>
+      </c>
+      <c r="H2140" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2140" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2140">
+        <v>2122465</v>
+      </c>
+      <c r="K2140">
+        <v>0</v>
+      </c>
+      <c r="L2140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2141" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2141">
+        <v>2023</v>
+      </c>
+      <c r="B2141" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2141" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2141" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2141" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2141">
+        <v>74519796</v>
+      </c>
+      <c r="G2141">
+        <v>2736680</v>
+      </c>
+      <c r="H2141" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2141" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2141">
+        <v>2736680</v>
+      </c>
+      <c r="K2141">
+        <v>0</v>
+      </c>
+      <c r="L2141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2142" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2142">
+        <v>2023</v>
+      </c>
+      <c r="B2142" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2142" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2142" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2142" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2142">
+        <v>26930343</v>
+      </c>
+      <c r="G2142">
+        <v>3370506</v>
+      </c>
+      <c r="H2142" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2142" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2142">
+        <v>3370506</v>
+      </c>
+      <c r="K2142">
+        <v>0</v>
+      </c>
+      <c r="L2142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2143" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2143">
+        <v>2023</v>
+      </c>
+      <c r="B2143" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2143" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2143">
+        <v>359616109</v>
+      </c>
+      <c r="E2143" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2143">
+        <v>51547086</v>
+      </c>
+      <c r="G2143">
+        <v>11609704</v>
+      </c>
+      <c r="H2143" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2143" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2143">
+        <v>11609704</v>
+      </c>
+      <c r="K2143">
+        <v>0</v>
+      </c>
+      <c r="L2143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2144" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2144">
+        <v>2023</v>
+      </c>
+      <c r="B2144" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2144" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2144">
+        <v>374163103</v>
+      </c>
+      <c r="E2144" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2144">
+        <v>97949141</v>
+      </c>
+      <c r="G2144">
+        <v>46202425</v>
+      </c>
+      <c r="H2144" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2144" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2144">
+        <v>46202425</v>
+      </c>
+      <c r="K2144">
+        <v>0</v>
+      </c>
+      <c r="L2144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2145" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2145">
+        <v>2023</v>
+      </c>
+      <c r="B2145" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2145" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2145" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2145" t="s">
+        <v>148</v>
+      </c>
+      <c r="F2145">
+        <v>56152697</v>
+      </c>
+      <c r="G2145">
+        <v>5587333</v>
+      </c>
+      <c r="H2145" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2145" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2145">
+        <v>5587333</v>
+      </c>
+      <c r="K2145">
+        <v>0</v>
+      </c>
+      <c r="L2145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2146" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2146">
+        <v>2023</v>
+      </c>
+      <c r="B2146" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2146" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2146" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2146" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2146">
+        <v>46217629</v>
+      </c>
+      <c r="G2146">
+        <v>5963565</v>
+      </c>
+      <c r="H2146" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2146" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2146">
+        <v>5963565</v>
+      </c>
+      <c r="K2146">
+        <v>0</v>
+      </c>
+      <c r="L2146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2147" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2147">
+        <v>2023</v>
+      </c>
+      <c r="B2147" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2147" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2147">
+        <v>449585108</v>
+      </c>
+      <c r="E2147" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2147">
+        <v>7828125</v>
+      </c>
+      <c r="G2147">
+        <v>937500</v>
+      </c>
+      <c r="H2147" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2147" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2147">
+        <v>937500</v>
+      </c>
+      <c r="K2147">
+        <v>0</v>
+      </c>
+      <c r="L2147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2148" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2148">
+        <v>2023</v>
+      </c>
+      <c r="B2148" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2148" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2148" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2148" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2148">
+        <v>211424711</v>
+      </c>
+      <c r="G2148">
+        <v>13322288</v>
+      </c>
+      <c r="H2148" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2148" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2148">
+        <v>13322288</v>
+      </c>
+      <c r="K2148">
+        <v>0</v>
+      </c>
+      <c r="L2148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2149" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2149">
+        <v>2023</v>
+      </c>
+      <c r="B2149" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2149" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2149" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2149" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2149">
+        <v>86689198</v>
+      </c>
+      <c r="G2149">
+        <v>4724207</v>
+      </c>
+      <c r="H2149" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2149" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2149">
+        <v>4724207</v>
+      </c>
+      <c r="K2149">
+        <v>0</v>
+      </c>
+      <c r="L2149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2150" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2150">
+        <v>2023</v>
+      </c>
+      <c r="B2150" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2150" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2150" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2150" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2150">
+        <v>48368986</v>
+      </c>
+      <c r="G2150">
+        <v>4417259</v>
+      </c>
+      <c r="H2150" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2150" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2150">
+        <v>4417259</v>
+      </c>
+      <c r="K2150">
+        <v>0</v>
+      </c>
+      <c r="L2150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2151" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2151">
+        <v>2023</v>
+      </c>
+      <c r="B2151" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2151" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2151" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2151" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2151">
+        <v>92389772</v>
+      </c>
+      <c r="G2151">
+        <v>9165652</v>
+      </c>
+      <c r="H2151" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2151" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2151">
+        <v>9165652</v>
+      </c>
+      <c r="K2151">
+        <v>0</v>
+      </c>
+      <c r="L2151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2152" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2152">
+        <v>2023</v>
+      </c>
+      <c r="B2152" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2152" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2152" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2152" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2152">
+        <v>420800369</v>
+      </c>
+      <c r="G2152">
+        <v>6264707</v>
+      </c>
+      <c r="H2152" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2152" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2152">
+        <v>6264707</v>
+      </c>
+      <c r="K2152">
+        <v>0</v>
+      </c>
+      <c r="L2152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2153" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2153">
+        <v>2023</v>
+      </c>
+      <c r="B2153" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2153" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2153">
+        <v>556099109</v>
+      </c>
+      <c r="E2153" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2153">
+        <v>1593720</v>
+      </c>
+      <c r="G2153">
+        <v>342000</v>
+      </c>
+      <c r="H2153" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2153" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2153">
+        <v>342000</v>
+      </c>
+      <c r="K2153">
+        <v>0</v>
+      </c>
+      <c r="L2153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2154" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2154">
+        <v>2023</v>
+      </c>
+      <c r="B2154" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2154" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2154">
+        <v>558868105</v>
+      </c>
+      <c r="E2154" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2154">
+        <v>29865180</v>
+      </c>
+      <c r="G2154">
+        <v>204500</v>
+      </c>
+      <c r="H2154" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2154" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2154">
+        <v>204500</v>
+      </c>
+      <c r="K2154">
+        <v>0</v>
+      </c>
+      <c r="L2154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2155" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2155">
+        <v>2023</v>
+      </c>
+      <c r="B2155" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2155" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2155">
+        <v>603170101</v>
+      </c>
+      <c r="E2155" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2155">
+        <v>30227307</v>
+      </c>
+      <c r="G2155">
+        <v>3178476</v>
+      </c>
+      <c r="H2155" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2155" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2155">
+        <v>3178476</v>
+      </c>
+      <c r="K2155">
+        <v>0</v>
+      </c>
+      <c r="L2155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2156" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2156">
+        <v>2023</v>
+      </c>
+      <c r="B2156" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2156" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2156" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2156" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2156">
+        <v>2964202</v>
+      </c>
+      <c r="G2156">
+        <v>1723373</v>
+      </c>
+      <c r="H2156" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2156" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2156">
+        <v>1723373</v>
+      </c>
+      <c r="K2156">
+        <v>0</v>
+      </c>
+      <c r="L2156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2157" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2157">
+        <v>2023</v>
+      </c>
+      <c r="B2157" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2157" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2157">
+        <v>640268108</v>
+      </c>
+      <c r="E2157" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2157">
+        <v>11137720</v>
+      </c>
+      <c r="G2157">
+        <v>18700000</v>
+      </c>
+      <c r="H2157" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2157" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2157">
+        <v>18700000</v>
+      </c>
+      <c r="K2157">
+        <v>0</v>
+      </c>
+      <c r="L2157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2158" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2158">
+        <v>2023</v>
+      </c>
+      <c r="B2158" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2158" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2158" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2158" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2158">
+        <v>83250000</v>
+      </c>
+      <c r="G2158">
+        <v>9000000</v>
+      </c>
+      <c r="H2158" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2158" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2158">
+        <v>9000000</v>
+      </c>
+      <c r="K2158">
+        <v>0</v>
+      </c>
+      <c r="L2158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2159" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2159">
+        <v>2023</v>
+      </c>
+      <c r="B2159" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2159" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2159" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2159" t="s">
+        <v>187</v>
+      </c>
+      <c r="F2159">
+        <v>10849129</v>
+      </c>
+      <c r="G2159">
+        <v>7805129</v>
+      </c>
+      <c r="H2159" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2159" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2159">
+        <v>7805129</v>
+      </c>
+      <c r="K2159">
+        <v>0</v>
+      </c>
+      <c r="L2159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2160" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2160">
+        <v>2023</v>
+      </c>
+      <c r="B2160" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2160" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2160">
+        <v>713317105</v>
+      </c>
+      <c r="E2160" t="s">
+        <v>189</v>
+      </c>
+      <c r="F2160">
+        <v>41310316</v>
+      </c>
+      <c r="G2160">
+        <v>8131952</v>
+      </c>
+      <c r="H2160" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2160" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2160">
+        <v>8131952</v>
+      </c>
+      <c r="K2160">
+        <v>0</v>
+      </c>
+      <c r="L2160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2161" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2161">
+        <v>2023</v>
+      </c>
+      <c r="B2161" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2161" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2161">
+        <v>729139105</v>
+      </c>
+      <c r="E2161" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2161">
+        <v>30553080</v>
+      </c>
+      <c r="G2161">
+        <v>1762000</v>
+      </c>
+      <c r="H2161" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2161" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2161">
+        <v>1762000</v>
+      </c>
+      <c r="K2161">
+        <v>0</v>
+      </c>
+      <c r="L2161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2162" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2162">
+        <v>2023</v>
+      </c>
+      <c r="B2162" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2162" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2162" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2162" t="s">
+        <v>194</v>
+      </c>
+      <c r="F2162">
+        <v>130123836</v>
+      </c>
+      <c r="G2162">
+        <v>5676067</v>
+      </c>
+      <c r="H2162" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2162" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2162">
+        <v>5676067</v>
+      </c>
+      <c r="K2162">
+        <v>0</v>
+      </c>
+      <c r="L2162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2163" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2163">
+        <v>2023</v>
+      </c>
+      <c r="B2163" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2163" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2163" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2163" t="s">
+        <v>197</v>
+      </c>
+      <c r="F2163">
+        <v>85142480</v>
+      </c>
+      <c r="G2163">
+        <v>3052796</v>
+      </c>
+      <c r="H2163" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2163" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2163">
+        <v>3052796</v>
+      </c>
+      <c r="K2163">
+        <v>0</v>
+      </c>
+      <c r="L2163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2164" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2164">
+        <v>2023</v>
+      </c>
+      <c r="B2164" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2164" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2164">
+        <v>834203309</v>
+      </c>
+      <c r="E2164" t="s">
+        <v>199</v>
+      </c>
+      <c r="F2164">
+        <v>36562890</v>
+      </c>
+      <c r="G2164">
+        <v>1239000</v>
+      </c>
+      <c r="H2164" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2164" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2164">
+        <v>1239000</v>
+      </c>
+      <c r="K2164">
+        <v>0</v>
+      </c>
+      <c r="L2164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2165" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2165">
+        <v>2023</v>
+      </c>
+      <c r="B2165" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2165" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2165" s="1">
+        <v>8.3422000000000001E+208</v>
+      </c>
+      <c r="E2165" t="s">
+        <v>201</v>
+      </c>
+      <c r="F2165">
+        <v>8634241</v>
+      </c>
+      <c r="G2165">
+        <v>3426286</v>
+      </c>
+      <c r="H2165" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2165" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2165">
+        <v>3426286</v>
+      </c>
+      <c r="K2165">
+        <v>0</v>
+      </c>
+      <c r="L2165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2166" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2166">
+        <v>2023</v>
+      </c>
+      <c r="B2166" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2166" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2166" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2166" t="s">
+        <v>204</v>
+      </c>
+      <c r="F2166">
+        <v>6753099</v>
+      </c>
+      <c r="G2166">
+        <v>2403238</v>
+      </c>
+      <c r="H2166" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2166" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2166">
+        <v>2403238</v>
+      </c>
+      <c r="K2166">
+        <v>0</v>
+      </c>
+      <c r="L2166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2167" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2167">
+        <v>2023</v>
+      </c>
+      <c r="B2167" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2167" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2167">
+        <v>877619106</v>
+      </c>
+      <c r="E2167" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2167">
+        <v>58373109</v>
+      </c>
+      <c r="G2167">
+        <v>18472503</v>
+      </c>
+      <c r="H2167" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2167" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2167">
+        <v>18472503</v>
+      </c>
+      <c r="K2167">
+        <v>0</v>
+      </c>
+      <c r="L2167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2168" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2168">
+        <v>2023</v>
+      </c>
+      <c r="B2168" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2168" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2168" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2168" t="s">
+        <v>209</v>
+      </c>
+      <c r="F2168">
+        <v>17132132</v>
+      </c>
+      <c r="G2168">
+        <v>6718483</v>
+      </c>
+      <c r="H2168" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2168" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2168">
+        <v>6718483</v>
+      </c>
+      <c r="K2168">
+        <v>0</v>
+      </c>
+      <c r="L2168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2169" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2169">
+        <v>2023</v>
+      </c>
+      <c r="B2169" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2169" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2169" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2169" t="s">
+        <v>212</v>
+      </c>
+      <c r="F2169">
+        <v>6146305</v>
+      </c>
+      <c r="G2169">
+        <v>961863</v>
+      </c>
+      <c r="H2169" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2169" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2169">
+        <v>961863</v>
+      </c>
+      <c r="K2169">
+        <v>0</v>
+      </c>
+      <c r="L2169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2170" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2170">
+        <v>2023</v>
+      </c>
+      <c r="B2170" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2170" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2170" t="s">
+        <v>214</v>
+      </c>
+      <c r="E2170" t="s">
+        <v>215</v>
+      </c>
+      <c r="F2170">
+        <v>99645972</v>
+      </c>
+      <c r="G2170">
+        <v>7236454</v>
+      </c>
+      <c r="H2170" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2170" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2170">
+        <v>7236454</v>
+      </c>
+      <c r="K2170">
+        <v>0</v>
+      </c>
+      <c r="L2170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2171" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2171">
+        <v>2023</v>
+      </c>
+      <c r="B2171" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2171" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2171" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2171" t="s">
+        <v>218</v>
+      </c>
+      <c r="F2171">
+        <v>2984792</v>
+      </c>
+      <c r="G2171">
+        <v>3470688</v>
+      </c>
+      <c r="H2171" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2171" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2171">
+        <v>3470688</v>
+      </c>
+      <c r="K2171">
+        <v>0</v>
+      </c>
+      <c r="L2171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2172" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2172">
+        <v>2023</v>
+      </c>
+      <c r="B2172" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2172" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2172" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2172" t="s">
+        <v>221</v>
+      </c>
+      <c r="F2172">
+        <v>20786595</v>
+      </c>
+      <c r="G2172">
+        <v>1483697</v>
+      </c>
+      <c r="H2172" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2172" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2172">
+        <v>1483697</v>
+      </c>
+      <c r="K2172">
+        <v>0</v>
+      </c>
+      <c r="L2172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2173" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2173">
+        <v>2023</v>
+      </c>
+      <c r="B2173" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2173" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2173" t="s">
+        <v>223</v>
+      </c>
+      <c r="E2173" t="s">
+        <v>224</v>
+      </c>
+      <c r="F2173">
+        <v>402296129</v>
+      </c>
+      <c r="G2173">
+        <v>7891254</v>
+      </c>
+      <c r="H2173" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2173" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2173">
+        <v>7891254</v>
+      </c>
+      <c r="K2173">
+        <v>0</v>
+      </c>
+      <c r="L2173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2174" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2174">
+        <v>2023</v>
+      </c>
+      <c r="B2174" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2174" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2174" t="s">
+        <v>226</v>
+      </c>
+      <c r="E2174" t="s">
+        <v>227</v>
+      </c>
+      <c r="F2174">
+        <v>30801892</v>
+      </c>
+      <c r="G2174">
+        <v>2007946</v>
+      </c>
+      <c r="H2174" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2174" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2174">
+        <v>2007946</v>
+      </c>
+      <c r="K2174">
+        <v>0</v>
+      </c>
+      <c r="L2174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2175" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2175">
+        <v>2023</v>
+      </c>
+      <c r="B2175" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2175" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2175" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2175" t="s">
+        <v>230</v>
+      </c>
+      <c r="F2175">
+        <v>98911552</v>
+      </c>
+      <c r="G2175">
+        <v>17202009</v>
+      </c>
+      <c r="H2175" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2175" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2175">
+        <v>17202009</v>
+      </c>
+      <c r="K2175">
+        <v>0</v>
+      </c>
+      <c r="L2175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2176" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2176">
+        <v>2023</v>
+      </c>
+      <c r="B2176" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2176" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2176" t="s">
+        <v>232</v>
+      </c>
+      <c r="E2176" t="s">
+        <v>233</v>
+      </c>
+      <c r="F2176">
+        <v>13150045</v>
+      </c>
+      <c r="G2176">
+        <v>6144881</v>
+      </c>
+      <c r="H2176" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2176" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2176">
+        <v>6144881</v>
+      </c>
+      <c r="K2176">
+        <v>0</v>
+      </c>
+      <c r="L2176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2177" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2177">
+        <v>2023</v>
+      </c>
+      <c r="B2177" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2177" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2177">
+        <v>929033108</v>
+      </c>
+      <c r="E2177" t="s">
+        <v>235</v>
+      </c>
+      <c r="F2177">
+        <v>48227626</v>
+      </c>
+      <c r="G2177">
+        <v>22748880</v>
+      </c>
+      <c r="H2177" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2177" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2177">
+        <v>22748880</v>
+      </c>
+      <c r="K2177">
+        <v>0</v>
+      </c>
+      <c r="L2177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2178" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2178">
+        <v>2023</v>
+      </c>
+      <c r="B2178" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2178" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2178" t="s">
+        <v>237</v>
+      </c>
+      <c r="E2178" t="s">
+        <v>238</v>
+      </c>
+      <c r="F2178">
+        <v>42129291</v>
+      </c>
+      <c r="G2178">
+        <v>1977901</v>
+      </c>
+      <c r="H2178" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2178" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2178">
+        <v>1977901</v>
+      </c>
+      <c r="K2178">
+        <v>0</v>
+      </c>
+      <c r="L2178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2179" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2179">
+        <v>2023</v>
+      </c>
+      <c r="B2179" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2179" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2179">
+        <v>925050106</v>
+      </c>
+      <c r="E2179" t="s">
+        <v>240</v>
+      </c>
+      <c r="F2179">
+        <v>102983237</v>
+      </c>
+      <c r="G2179">
+        <v>6317990</v>
+      </c>
+      <c r="H2179" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2179" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2179">
+        <v>6317990</v>
+      </c>
+      <c r="K2179">
+        <v>0</v>
+      </c>
+      <c r="L2179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2180" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2180">
+        <v>2023</v>
+      </c>
+      <c r="B2180" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2180" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2180" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2180" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2180">
+        <v>633333</v>
+      </c>
+      <c r="G2180">
+        <v>333333</v>
+      </c>
+      <c r="H2180" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2180" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2180">
+        <v>333333</v>
+      </c>
+      <c r="K2180">
+        <v>0</v>
+      </c>
+      <c r="L2180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2181" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2181">
+        <v>2023</v>
+      </c>
+      <c r="B2181" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2181" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2181" t="s">
+        <v>245</v>
+      </c>
+      <c r="E2181" t="s">
+        <v>246</v>
+      </c>
+      <c r="F2181">
+        <v>37587910</v>
+      </c>
+      <c r="G2181">
+        <v>6809404</v>
+      </c>
+      <c r="H2181" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2181" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2181">
+        <v>6809404</v>
+      </c>
+      <c r="K2181">
+        <v>0</v>
+      </c>
+      <c r="L2181">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made loop functional and added share value
</commit_message>
<xml_diff>
--- a/Master.xlsx
+++ b/Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasg17/Documents/GitHub/Health-Innovation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4570DAD8-6CD4-2742-8BFB-FD049E503B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCA55DBE-A60F-F94C-A146-6DCC519E866B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="760" windowWidth="28060" windowHeight="17440" xr2:uid="{7B871D28-6C56-6A4C-8DC7-F3E0A8269B8A}"/>
+    <workbookView xWindow="3560" yWindow="760" windowWidth="28060" windowHeight="17440" activeTab="1" xr2:uid="{7B871D28-6C56-6A4C-8DC7-F3E0A8269B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="RA CAPITAL MANAGEMENT, L.P." sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11135" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11482" uniqueCount="852">
   <si>
     <t>COM NEW</t>
   </si>
@@ -2944,9 +2944,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DBE7DD-EA50-0848-ABCD-4874656132C1}">
-  <dimension ref="A1:L2496"/>
+  <dimension ref="A1:L2562"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2394" workbookViewId="0"/>
+    <sheetView topLeftCell="A2551" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -83810,6 +83810,732 @@
       </c>
       <c r="C2496">
         <v>18741887</v>
+      </c>
+    </row>
+    <row r="2497" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2497">
+        <v>2023</v>
+      </c>
+      <c r="B2497" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2497">
+        <v>52997676</v>
+      </c>
+    </row>
+    <row r="2498" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2498">
+        <v>2023</v>
+      </c>
+      <c r="B2498" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2498">
+        <v>176277677</v>
+      </c>
+    </row>
+    <row r="2499" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2499">
+        <v>2023</v>
+      </c>
+      <c r="B2499" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2499">
+        <v>30129403</v>
+      </c>
+    </row>
+    <row r="2500" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2500">
+        <v>2023</v>
+      </c>
+      <c r="B2500" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2500">
+        <v>45988456</v>
+      </c>
+    </row>
+    <row r="2501" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2501">
+        <v>2023</v>
+      </c>
+      <c r="B2501" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2501">
+        <v>61968061</v>
+      </c>
+    </row>
+    <row r="2502" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2502">
+        <v>2023</v>
+      </c>
+      <c r="B2502" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2502">
+        <v>112142236</v>
+      </c>
+    </row>
+    <row r="2503" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2503">
+        <v>2023</v>
+      </c>
+      <c r="B2503" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2503">
+        <v>53713988</v>
+      </c>
+    </row>
+    <row r="2504" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2504">
+        <v>2023</v>
+      </c>
+      <c r="B2504" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2504">
+        <v>89264824</v>
+      </c>
+    </row>
+    <row r="2505" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2505">
+        <v>2023</v>
+      </c>
+      <c r="B2505" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2505">
+        <v>35757583</v>
+      </c>
+    </row>
+    <row r="2506" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2506">
+        <v>2023</v>
+      </c>
+      <c r="B2506" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2506">
+        <v>1003779130</v>
+      </c>
+    </row>
+    <row r="2507" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2507">
+        <v>2023</v>
+      </c>
+      <c r="B2507" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2507">
+        <v>40940447</v>
+      </c>
+    </row>
+    <row r="2508" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2508">
+        <v>2023</v>
+      </c>
+      <c r="B2508" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2508">
+        <v>69890000</v>
+      </c>
+    </row>
+    <row r="2509" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2509">
+        <v>2023</v>
+      </c>
+      <c r="B2509" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2509">
+        <v>16072000</v>
+      </c>
+    </row>
+    <row r="2510" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2510">
+        <v>2023</v>
+      </c>
+      <c r="B2510" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2510">
+        <v>136958573</v>
+      </c>
+    </row>
+    <row r="2511" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2511">
+        <v>2023</v>
+      </c>
+      <c r="B2511" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2511">
+        <v>10118914</v>
+      </c>
+    </row>
+    <row r="2512" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2512">
+        <v>2023</v>
+      </c>
+      <c r="B2512" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2512">
+        <v>12796009</v>
+      </c>
+    </row>
+    <row r="2513" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2513">
+        <v>2023</v>
+      </c>
+      <c r="B2513" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2513">
+        <v>6240259</v>
+      </c>
+    </row>
+    <row r="2514" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2514">
+        <v>2023</v>
+      </c>
+      <c r="B2514" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2514">
+        <v>62557433</v>
+      </c>
+    </row>
+    <row r="2515" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2515">
+        <v>2023</v>
+      </c>
+      <c r="B2515" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2515">
+        <v>5725631</v>
+      </c>
+    </row>
+    <row r="2516" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2516">
+        <v>2023</v>
+      </c>
+      <c r="B2516" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2516">
+        <v>9516400</v>
+      </c>
+    </row>
+    <row r="2517" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2517">
+        <v>2023</v>
+      </c>
+      <c r="B2517" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2517">
+        <v>72427670</v>
+      </c>
+    </row>
+    <row r="2518" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2518">
+        <v>2023</v>
+      </c>
+      <c r="B2518" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2518">
+        <v>103475400</v>
+      </c>
+    </row>
+    <row r="2519" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2519">
+        <v>2023</v>
+      </c>
+      <c r="B2519" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2519">
+        <v>95826884</v>
+      </c>
+    </row>
+    <row r="2520" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2520">
+        <v>2023</v>
+      </c>
+      <c r="B2520" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2520">
+        <v>34586733</v>
+      </c>
+    </row>
+    <row r="2521" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2521">
+        <v>2023</v>
+      </c>
+      <c r="B2521" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2521">
+        <v>28992872</v>
+      </c>
+    </row>
+    <row r="2522" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2522">
+        <v>2023</v>
+      </c>
+      <c r="B2522" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2522">
+        <v>74519796</v>
+      </c>
+    </row>
+    <row r="2523" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2523">
+        <v>2023</v>
+      </c>
+      <c r="B2523" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2523">
+        <v>26930343</v>
+      </c>
+    </row>
+    <row r="2524" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2524">
+        <v>2023</v>
+      </c>
+      <c r="B2524" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2524">
+        <v>51547086</v>
+      </c>
+    </row>
+    <row r="2525" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2525">
+        <v>2023</v>
+      </c>
+      <c r="B2525" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2525">
+        <v>97949141</v>
+      </c>
+    </row>
+    <row r="2526" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2526">
+        <v>2023</v>
+      </c>
+      <c r="B2526" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2526">
+        <v>56152697</v>
+      </c>
+    </row>
+    <row r="2527" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2527">
+        <v>2023</v>
+      </c>
+      <c r="B2527" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2527">
+        <v>46217629</v>
+      </c>
+    </row>
+    <row r="2528" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2528">
+        <v>2023</v>
+      </c>
+      <c r="B2528" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2528">
+        <v>7828125</v>
+      </c>
+    </row>
+    <row r="2529" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2529">
+        <v>2023</v>
+      </c>
+      <c r="B2529" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2529">
+        <v>211424711</v>
+      </c>
+    </row>
+    <row r="2530" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2530">
+        <v>2023</v>
+      </c>
+      <c r="B2530" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2530">
+        <v>86689198</v>
+      </c>
+    </row>
+    <row r="2531" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2531">
+        <v>2023</v>
+      </c>
+      <c r="B2531" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2531">
+        <v>48368986</v>
+      </c>
+    </row>
+    <row r="2532" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2532">
+        <v>2023</v>
+      </c>
+      <c r="B2532" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2532">
+        <v>92389772</v>
+      </c>
+    </row>
+    <row r="2533" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2533">
+        <v>2023</v>
+      </c>
+      <c r="B2533" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2533">
+        <v>420800369</v>
+      </c>
+    </row>
+    <row r="2534" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2534">
+        <v>2023</v>
+      </c>
+      <c r="B2534" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2534">
+        <v>1593720</v>
+      </c>
+    </row>
+    <row r="2535" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2535">
+        <v>2023</v>
+      </c>
+      <c r="B2535" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2535">
+        <v>29865180</v>
+      </c>
+    </row>
+    <row r="2536" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2536">
+        <v>2023</v>
+      </c>
+      <c r="B2536" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2536">
+        <v>30227307</v>
+      </c>
+    </row>
+    <row r="2537" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2537">
+        <v>2023</v>
+      </c>
+      <c r="B2537" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2537">
+        <v>2964202</v>
+      </c>
+    </row>
+    <row r="2538" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2538">
+        <v>2023</v>
+      </c>
+      <c r="B2538" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2538">
+        <v>11137720</v>
+      </c>
+    </row>
+    <row r="2539" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2539">
+        <v>2023</v>
+      </c>
+      <c r="B2539" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2539">
+        <v>83250000</v>
+      </c>
+    </row>
+    <row r="2540" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2540">
+        <v>2023</v>
+      </c>
+      <c r="B2540" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2540">
+        <v>10849129</v>
+      </c>
+    </row>
+    <row r="2541" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2541">
+        <v>2023</v>
+      </c>
+      <c r="B2541" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2541">
+        <v>41310316</v>
+      </c>
+    </row>
+    <row r="2542" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2542">
+        <v>2023</v>
+      </c>
+      <c r="B2542" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2542">
+        <v>30553080</v>
+      </c>
+    </row>
+    <row r="2543" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2543">
+        <v>2023</v>
+      </c>
+      <c r="B2543" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2543">
+        <v>130123836</v>
+      </c>
+    </row>
+    <row r="2544" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2544">
+        <v>2023</v>
+      </c>
+      <c r="B2544" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2544">
+        <v>85142480</v>
+      </c>
+    </row>
+    <row r="2545" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2545">
+        <v>2023</v>
+      </c>
+      <c r="B2545" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2545">
+        <v>36562890</v>
+      </c>
+    </row>
+    <row r="2546" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2546">
+        <v>2023</v>
+      </c>
+      <c r="B2546" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2546">
+        <v>8634241</v>
+      </c>
+    </row>
+    <row r="2547" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2547">
+        <v>2023</v>
+      </c>
+      <c r="B2547" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2547">
+        <v>6753099</v>
+      </c>
+    </row>
+    <row r="2548" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2548">
+        <v>2023</v>
+      </c>
+      <c r="B2548" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2548">
+        <v>58373109</v>
+      </c>
+    </row>
+    <row r="2549" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2549">
+        <v>2023</v>
+      </c>
+      <c r="B2549" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2549">
+        <v>17132132</v>
+      </c>
+    </row>
+    <row r="2550" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2550">
+        <v>2023</v>
+      </c>
+      <c r="B2550" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2550">
+        <v>6146305</v>
+      </c>
+    </row>
+    <row r="2551" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2551">
+        <v>2023</v>
+      </c>
+      <c r="B2551" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2551">
+        <v>99645972</v>
+      </c>
+    </row>
+    <row r="2552" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2552">
+        <v>2023</v>
+      </c>
+      <c r="B2552" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2552">
+        <v>2984792</v>
+      </c>
+    </row>
+    <row r="2553" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2553">
+        <v>2023</v>
+      </c>
+      <c r="B2553" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2553">
+        <v>20786595</v>
+      </c>
+    </row>
+    <row r="2554" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2554">
+        <v>2023</v>
+      </c>
+      <c r="B2554" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2554">
+        <v>402296129</v>
+      </c>
+    </row>
+    <row r="2555" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2555">
+        <v>2023</v>
+      </c>
+      <c r="B2555" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2555">
+        <v>30801892</v>
+      </c>
+    </row>
+    <row r="2556" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2556">
+        <v>2023</v>
+      </c>
+      <c r="B2556" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2556">
+        <v>98911552</v>
+      </c>
+    </row>
+    <row r="2557" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2557">
+        <v>2023</v>
+      </c>
+      <c r="B2557" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2557">
+        <v>13150045</v>
+      </c>
+    </row>
+    <row r="2558" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2558">
+        <v>2023</v>
+      </c>
+      <c r="B2558" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2558">
+        <v>48227626</v>
+      </c>
+    </row>
+    <row r="2559" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2559">
+        <v>2023</v>
+      </c>
+      <c r="B2559" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2559">
+        <v>42129291</v>
+      </c>
+    </row>
+    <row r="2560" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2560">
+        <v>2023</v>
+      </c>
+      <c r="B2560" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2560">
+        <v>102983237</v>
+      </c>
+    </row>
+    <row r="2561" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2561">
+        <v>2023</v>
+      </c>
+      <c r="B2561" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2561">
+        <v>633333</v>
+      </c>
+    </row>
+    <row r="2562" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2562">
+        <v>2023</v>
+      </c>
+      <c r="B2562" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2562">
+        <v>37587910</v>
       </c>
     </row>
   </sheetData>
@@ -83819,9 +84545,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF1BB6E-2638-6F4C-AE3A-D3BA1AF8B8FD}">
-  <dimension ref="A1:C239"/>
+  <dimension ref="A1:D520"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A469" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -86454,6 +87180,3226 @@
         <v>38035</v>
       </c>
     </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>2022</v>
+      </c>
+      <c r="B240" t="s">
+        <v>829</v>
+      </c>
+      <c r="C240">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>2022</v>
+      </c>
+      <c r="B241" t="s">
+        <v>23</v>
+      </c>
+      <c r="C241">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>2022</v>
+      </c>
+      <c r="B242" t="s">
+        <v>830</v>
+      </c>
+      <c r="C242">
+        <v>21098</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>2022</v>
+      </c>
+      <c r="B243" t="s">
+        <v>831</v>
+      </c>
+      <c r="C243">
+        <v>10420</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>2022</v>
+      </c>
+      <c r="B244" t="s">
+        <v>829</v>
+      </c>
+      <c r="C244">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>2022</v>
+      </c>
+      <c r="B245" t="s">
+        <v>23</v>
+      </c>
+      <c r="C245">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>2022</v>
+      </c>
+      <c r="B246" t="s">
+        <v>830</v>
+      </c>
+      <c r="C246">
+        <v>15220</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>2022</v>
+      </c>
+      <c r="B247" t="s">
+        <v>831</v>
+      </c>
+      <c r="C247">
+        <v>10152</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>2022</v>
+      </c>
+      <c r="B248" t="s">
+        <v>832</v>
+      </c>
+      <c r="C248">
+        <v>17933</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>2022</v>
+      </c>
+      <c r="B249" t="s">
+        <v>829</v>
+      </c>
+      <c r="C249">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>2022</v>
+      </c>
+      <c r="B250" t="s">
+        <v>23</v>
+      </c>
+      <c r="C250">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>2022</v>
+      </c>
+      <c r="B251" t="s">
+        <v>830</v>
+      </c>
+      <c r="C251">
+        <v>40248</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>2022</v>
+      </c>
+      <c r="B252" t="s">
+        <v>831</v>
+      </c>
+      <c r="C252">
+        <v>20989</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>2022</v>
+      </c>
+      <c r="B253" t="s">
+        <v>832</v>
+      </c>
+      <c r="C253">
+        <v>20694</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>2022</v>
+      </c>
+      <c r="B254" t="s">
+        <v>829</v>
+      </c>
+      <c r="C254">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>2022</v>
+      </c>
+      <c r="B255" t="s">
+        <v>23</v>
+      </c>
+      <c r="C255">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>2022</v>
+      </c>
+      <c r="B256" t="s">
+        <v>3</v>
+      </c>
+      <c r="C256">
+        <v>27149</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>2022</v>
+      </c>
+      <c r="B257" t="s">
+        <v>830</v>
+      </c>
+      <c r="C257">
+        <v>55888</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>2022</v>
+      </c>
+      <c r="B258" t="s">
+        <v>831</v>
+      </c>
+      <c r="C258">
+        <v>22909</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>2022</v>
+      </c>
+      <c r="B259" t="s">
+        <v>832</v>
+      </c>
+      <c r="C259">
+        <v>47480</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>2021</v>
+      </c>
+      <c r="B260" t="s">
+        <v>829</v>
+      </c>
+      <c r="C260">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>2021</v>
+      </c>
+      <c r="B261" t="s">
+        <v>833</v>
+      </c>
+      <c r="C261">
+        <v>15289</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>2021</v>
+      </c>
+      <c r="B262" t="s">
+        <v>23</v>
+      </c>
+      <c r="C262">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>2021</v>
+      </c>
+      <c r="B263" t="s">
+        <v>3</v>
+      </c>
+      <c r="C263">
+        <v>34466</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>2021</v>
+      </c>
+      <c r="B264" t="s">
+        <v>830</v>
+      </c>
+      <c r="C264">
+        <v>59742</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>2021</v>
+      </c>
+      <c r="B265" t="s">
+        <v>834</v>
+      </c>
+      <c r="C265">
+        <v>42859</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>2021</v>
+      </c>
+      <c r="B266" t="s">
+        <v>832</v>
+      </c>
+      <c r="C266">
+        <v>45209</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>2021</v>
+      </c>
+      <c r="B267" t="s">
+        <v>835</v>
+      </c>
+      <c r="C267">
+        <v>4203</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>2021</v>
+      </c>
+      <c r="B268" t="s">
+        <v>829</v>
+      </c>
+      <c r="C268">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>2021</v>
+      </c>
+      <c r="B269" t="s">
+        <v>833</v>
+      </c>
+      <c r="C269">
+        <v>16473</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>2021</v>
+      </c>
+      <c r="B270" t="s">
+        <v>23</v>
+      </c>
+      <c r="C270">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <v>2021</v>
+      </c>
+      <c r="B271" t="s">
+        <v>3</v>
+      </c>
+      <c r="C271">
+        <v>33918</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>2021</v>
+      </c>
+      <c r="B272" t="s">
+        <v>830</v>
+      </c>
+      <c r="C272">
+        <v>58147</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>2021</v>
+      </c>
+      <c r="B273" t="s">
+        <v>834</v>
+      </c>
+      <c r="C273">
+        <v>37574</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>2021</v>
+      </c>
+      <c r="B274" t="s">
+        <v>836</v>
+      </c>
+      <c r="C274">
+        <v>79809</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>2021</v>
+      </c>
+      <c r="B275" t="s">
+        <v>829</v>
+      </c>
+      <c r="C275">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>2021</v>
+      </c>
+      <c r="B276" t="s">
+        <v>833</v>
+      </c>
+      <c r="C276">
+        <v>20176</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>2021</v>
+      </c>
+      <c r="B277" t="s">
+        <v>23</v>
+      </c>
+      <c r="C277">
+        <v>2682</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <v>2021</v>
+      </c>
+      <c r="B278" t="s">
+        <v>4</v>
+      </c>
+      <c r="C278">
+        <v>3491</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>2021</v>
+      </c>
+      <c r="B279" t="s">
+        <v>3</v>
+      </c>
+      <c r="C279">
+        <v>41527</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>2021</v>
+      </c>
+      <c r="B280" t="s">
+        <v>830</v>
+      </c>
+      <c r="C280">
+        <v>57209</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <v>2021</v>
+      </c>
+      <c r="B281" t="s">
+        <v>834</v>
+      </c>
+      <c r="C281">
+        <v>33186</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A282">
+        <v>2021</v>
+      </c>
+      <c r="B282" t="s">
+        <v>836</v>
+      </c>
+      <c r="C282">
+        <v>107033</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A283">
+        <v>2021</v>
+      </c>
+      <c r="B283" t="s">
+        <v>837</v>
+      </c>
+      <c r="C283">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A284">
+        <v>2021</v>
+      </c>
+      <c r="B284" t="s">
+        <v>6</v>
+      </c>
+      <c r="C284">
+        <v>25679</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A285">
+        <v>2021</v>
+      </c>
+      <c r="B285" t="s">
+        <v>833</v>
+      </c>
+      <c r="C285">
+        <v>25679</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A286">
+        <v>2021</v>
+      </c>
+      <c r="B286" t="s">
+        <v>23</v>
+      </c>
+      <c r="C286">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A287">
+        <v>2021</v>
+      </c>
+      <c r="B287" t="s">
+        <v>4</v>
+      </c>
+      <c r="C287">
+        <v>16612</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A288">
+        <v>2021</v>
+      </c>
+      <c r="B288" t="s">
+        <v>3</v>
+      </c>
+      <c r="C288">
+        <v>39611</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A289">
+        <v>2021</v>
+      </c>
+      <c r="B289" t="s">
+        <v>830</v>
+      </c>
+      <c r="C289">
+        <v>34379</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A290">
+        <v>2021</v>
+      </c>
+      <c r="B290" t="s">
+        <v>834</v>
+      </c>
+      <c r="C290">
+        <v>21175</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A291">
+        <v>2021</v>
+      </c>
+      <c r="B291" t="s">
+        <v>838</v>
+      </c>
+      <c r="C291">
+        <v>42115</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A292">
+        <v>2020</v>
+      </c>
+      <c r="B292" t="s">
+        <v>837</v>
+      </c>
+      <c r="C292">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A293">
+        <v>2020</v>
+      </c>
+      <c r="B293" t="s">
+        <v>7</v>
+      </c>
+      <c r="C293">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A294">
+        <v>2020</v>
+      </c>
+      <c r="B294" t="s">
+        <v>6</v>
+      </c>
+      <c r="C294">
+        <v>21650</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A295">
+        <v>2020</v>
+      </c>
+      <c r="B295" t="s">
+        <v>833</v>
+      </c>
+      <c r="C295">
+        <v>23083</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A296">
+        <v>2020</v>
+      </c>
+      <c r="B296" t="s">
+        <v>23</v>
+      </c>
+      <c r="C296">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A297">
+        <v>2020</v>
+      </c>
+      <c r="B297" t="s">
+        <v>4</v>
+      </c>
+      <c r="C297">
+        <v>16095</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A298">
+        <v>2020</v>
+      </c>
+      <c r="B298" t="s">
+        <v>3</v>
+      </c>
+      <c r="C298">
+        <v>18337</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A299">
+        <v>2020</v>
+      </c>
+      <c r="B299" t="s">
+        <v>830</v>
+      </c>
+      <c r="C299">
+        <v>36486</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A300">
+        <v>2020</v>
+      </c>
+      <c r="B300" t="s">
+        <v>834</v>
+      </c>
+      <c r="C300">
+        <v>19894</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A301">
+        <v>2020</v>
+      </c>
+      <c r="B301" t="s">
+        <v>838</v>
+      </c>
+      <c r="C301">
+        <v>57779</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <v>2020</v>
+      </c>
+      <c r="B302" t="s">
+        <v>837</v>
+      </c>
+      <c r="C302">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A303">
+        <v>2020</v>
+      </c>
+      <c r="B303" t="s">
+        <v>8</v>
+      </c>
+      <c r="C303">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A304">
+        <v>2020</v>
+      </c>
+      <c r="B304" t="s">
+        <v>7</v>
+      </c>
+      <c r="C304">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A305">
+        <v>2020</v>
+      </c>
+      <c r="B305" t="s">
+        <v>6</v>
+      </c>
+      <c r="C305">
+        <v>20806</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A306">
+        <v>2020</v>
+      </c>
+      <c r="B306" t="s">
+        <v>833</v>
+      </c>
+      <c r="C306">
+        <v>26871</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A307">
+        <v>2020</v>
+      </c>
+      <c r="B307" t="s">
+        <v>23</v>
+      </c>
+      <c r="C307">
+        <v>2904</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A308">
+        <v>2020</v>
+      </c>
+      <c r="B308" t="s">
+        <v>4</v>
+      </c>
+      <c r="C308">
+        <v>21570</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A309">
+        <v>2020</v>
+      </c>
+      <c r="B309" t="s">
+        <v>3</v>
+      </c>
+      <c r="C309">
+        <v>14158</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A310">
+        <v>2020</v>
+      </c>
+      <c r="B310" t="s">
+        <v>830</v>
+      </c>
+      <c r="C310">
+        <v>30147</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A311">
+        <v>2020</v>
+      </c>
+      <c r="B311" t="s">
+        <v>834</v>
+      </c>
+      <c r="C311">
+        <v>23014</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A312">
+        <v>2020</v>
+      </c>
+      <c r="B312" t="s">
+        <v>837</v>
+      </c>
+      <c r="C312">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A313">
+        <v>2020</v>
+      </c>
+      <c r="B313" t="s">
+        <v>8</v>
+      </c>
+      <c r="C313">
+        <v>3110</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A314">
+        <v>2020</v>
+      </c>
+      <c r="B314" t="s">
+        <v>7</v>
+      </c>
+      <c r="C314">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A315">
+        <v>2020</v>
+      </c>
+      <c r="B315" t="s">
+        <v>6</v>
+      </c>
+      <c r="C315">
+        <v>13155</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A316">
+        <v>2020</v>
+      </c>
+      <c r="B316" t="s">
+        <v>833</v>
+      </c>
+      <c r="C316">
+        <v>18525</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A317">
+        <v>2020</v>
+      </c>
+      <c r="B317" t="s">
+        <v>23</v>
+      </c>
+      <c r="C317">
+        <v>3115</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A318">
+        <v>2020</v>
+      </c>
+      <c r="B318" t="s">
+        <v>4</v>
+      </c>
+      <c r="C318">
+        <v>19234</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A319">
+        <v>2020</v>
+      </c>
+      <c r="B319" t="s">
+        <v>3</v>
+      </c>
+      <c r="C319">
+        <v>18610</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A320">
+        <v>2020</v>
+      </c>
+      <c r="B320" t="s">
+        <v>830</v>
+      </c>
+      <c r="C320">
+        <v>26143</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A321">
+        <v>2020</v>
+      </c>
+      <c r="B321" t="s">
+        <v>834</v>
+      </c>
+      <c r="C321">
+        <v>15976</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A322">
+        <v>2020</v>
+      </c>
+      <c r="B322" t="s">
+        <v>837</v>
+      </c>
+      <c r="C322">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A323">
+        <v>2020</v>
+      </c>
+      <c r="B323" t="s">
+        <v>8</v>
+      </c>
+      <c r="C323">
+        <v>2482</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A324">
+        <v>2020</v>
+      </c>
+      <c r="B324" t="s">
+        <v>7</v>
+      </c>
+      <c r="C324">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A325">
+        <v>2020</v>
+      </c>
+      <c r="B325" t="s">
+        <v>6</v>
+      </c>
+      <c r="C325">
+        <v>30625</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A326">
+        <v>2020</v>
+      </c>
+      <c r="B326" t="s">
+        <v>833</v>
+      </c>
+      <c r="C326">
+        <v>28005</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A327">
+        <v>2020</v>
+      </c>
+      <c r="B327" t="s">
+        <v>23</v>
+      </c>
+      <c r="C327">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A328">
+        <v>2020</v>
+      </c>
+      <c r="B328" t="s">
+        <v>4</v>
+      </c>
+      <c r="C328">
+        <v>28528</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A329">
+        <v>2020</v>
+      </c>
+      <c r="B329" t="s">
+        <v>3</v>
+      </c>
+      <c r="C329">
+        <v>20070</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A330">
+        <v>2020</v>
+      </c>
+      <c r="B330" t="s">
+        <v>830</v>
+      </c>
+      <c r="C330">
+        <v>18061</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A331">
+        <v>2020</v>
+      </c>
+      <c r="B331" t="s">
+        <v>834</v>
+      </c>
+      <c r="C331">
+        <v>31562</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A332">
+        <v>2019</v>
+      </c>
+      <c r="B332" t="s">
+        <v>837</v>
+      </c>
+      <c r="C332">
+        <v>4112</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A333">
+        <v>2019</v>
+      </c>
+      <c r="B333" t="s">
+        <v>8</v>
+      </c>
+      <c r="C333">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A334">
+        <v>2019</v>
+      </c>
+      <c r="B334" t="s">
+        <v>7</v>
+      </c>
+      <c r="C334">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A335">
+        <v>2019</v>
+      </c>
+      <c r="B335" t="s">
+        <v>6</v>
+      </c>
+      <c r="C335">
+        <v>19947</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A336">
+        <v>2019</v>
+      </c>
+      <c r="B336" t="s">
+        <v>833</v>
+      </c>
+      <c r="C336">
+        <v>18401</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A337">
+        <v>2019</v>
+      </c>
+      <c r="B337" t="s">
+        <v>23</v>
+      </c>
+      <c r="C337">
+        <v>3957</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A338">
+        <v>2019</v>
+      </c>
+      <c r="B338" t="s">
+        <v>4</v>
+      </c>
+      <c r="C338">
+        <v>20010</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A339">
+        <v>2019</v>
+      </c>
+      <c r="B339" t="s">
+        <v>3</v>
+      </c>
+      <c r="C339">
+        <v>16584</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A340">
+        <v>2019</v>
+      </c>
+      <c r="B340" t="s">
+        <v>830</v>
+      </c>
+      <c r="C340">
+        <v>21815</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A341">
+        <v>2019</v>
+      </c>
+      <c r="B341" t="s">
+        <v>834</v>
+      </c>
+      <c r="C341">
+        <v>34089</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A342">
+        <v>2019</v>
+      </c>
+      <c r="B342" t="s">
+        <v>837</v>
+      </c>
+      <c r="C342">
+        <v>9019</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A343">
+        <v>2019</v>
+      </c>
+      <c r="B343" t="s">
+        <v>8</v>
+      </c>
+      <c r="C343">
+        <v>2764</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A344">
+        <v>2019</v>
+      </c>
+      <c r="B344" t="s">
+        <v>7</v>
+      </c>
+      <c r="C344">
+        <v>2306</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A345">
+        <v>2019</v>
+      </c>
+      <c r="B345" t="s">
+        <v>6</v>
+      </c>
+      <c r="C345">
+        <v>38088</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A346">
+        <v>2019</v>
+      </c>
+      <c r="B346" t="s">
+        <v>833</v>
+      </c>
+      <c r="C346">
+        <v>20709</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A347">
+        <v>2019</v>
+      </c>
+      <c r="B347" t="s">
+        <v>23</v>
+      </c>
+      <c r="C347">
+        <v>4672</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A348">
+        <v>2019</v>
+      </c>
+      <c r="B348" t="s">
+        <v>4</v>
+      </c>
+      <c r="C348">
+        <v>31393</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A349">
+        <v>2019</v>
+      </c>
+      <c r="B349" t="s">
+        <v>3</v>
+      </c>
+      <c r="C349">
+        <v>20763</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A350">
+        <v>2019</v>
+      </c>
+      <c r="B350" t="s">
+        <v>830</v>
+      </c>
+      <c r="C350">
+        <v>19268</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A351">
+        <v>2019</v>
+      </c>
+      <c r="B351" t="s">
+        <v>837</v>
+      </c>
+      <c r="C351">
+        <v>15784</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A352">
+        <v>2019</v>
+      </c>
+      <c r="B352" t="s">
+        <v>8</v>
+      </c>
+      <c r="C352">
+        <v>2494</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A353">
+        <v>2019</v>
+      </c>
+      <c r="B353" t="s">
+        <v>7</v>
+      </c>
+      <c r="C353">
+        <v>2263</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A354">
+        <v>2019</v>
+      </c>
+      <c r="B354" t="s">
+        <v>6</v>
+      </c>
+      <c r="C354">
+        <v>52419</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A355">
+        <v>2019</v>
+      </c>
+      <c r="B355" t="s">
+        <v>833</v>
+      </c>
+      <c r="C355">
+        <v>28739</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A356">
+        <v>2019</v>
+      </c>
+      <c r="B356" t="s">
+        <v>839</v>
+      </c>
+      <c r="C356">
+        <v>5423</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A357">
+        <v>2019</v>
+      </c>
+      <c r="B357" t="s">
+        <v>4</v>
+      </c>
+      <c r="C357">
+        <v>42572</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A358">
+        <v>2019</v>
+      </c>
+      <c r="B358" t="s">
+        <v>3</v>
+      </c>
+      <c r="C358">
+        <v>20781</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A359">
+        <v>2019</v>
+      </c>
+      <c r="B359" t="s">
+        <v>837</v>
+      </c>
+      <c r="C359">
+        <v>14988</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A360">
+        <v>2019</v>
+      </c>
+      <c r="B360" t="s">
+        <v>8</v>
+      </c>
+      <c r="C360">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A361">
+        <v>2019</v>
+      </c>
+      <c r="B361" t="s">
+        <v>7</v>
+      </c>
+      <c r="C361">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A362">
+        <v>2019</v>
+      </c>
+      <c r="B362" t="s">
+        <v>6</v>
+      </c>
+      <c r="C362">
+        <v>50327</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A363">
+        <v>2019</v>
+      </c>
+      <c r="B363" t="s">
+        <v>833</v>
+      </c>
+      <c r="C363">
+        <v>27019</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A364">
+        <v>2019</v>
+      </c>
+      <c r="B364" t="s">
+        <v>840</v>
+      </c>
+      <c r="C364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A365">
+        <v>2019</v>
+      </c>
+      <c r="B365" t="s">
+        <v>841</v>
+      </c>
+      <c r="C365">
+        <v>4336</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A366">
+        <v>2019</v>
+      </c>
+      <c r="B366" t="s">
+        <v>4</v>
+      </c>
+      <c r="C366">
+        <v>45555</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A367">
+        <v>2019</v>
+      </c>
+      <c r="B367" t="s">
+        <v>3</v>
+      </c>
+      <c r="C367">
+        <v>16457</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A368">
+        <v>2018</v>
+      </c>
+      <c r="B368" t="s">
+        <v>837</v>
+      </c>
+      <c r="C368">
+        <v>38465</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A369">
+        <v>2018</v>
+      </c>
+      <c r="B369" t="s">
+        <v>8</v>
+      </c>
+      <c r="C369">
+        <v>4974</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A370">
+        <v>2018</v>
+      </c>
+      <c r="B370" t="s">
+        <v>7</v>
+      </c>
+      <c r="C370">
+        <v>2286</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A371">
+        <v>2018</v>
+      </c>
+      <c r="B371" t="s">
+        <v>6</v>
+      </c>
+      <c r="C371">
+        <v>57033</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A372">
+        <v>2018</v>
+      </c>
+      <c r="B372" t="s">
+        <v>833</v>
+      </c>
+      <c r="C372">
+        <v>66455</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A373">
+        <v>2018</v>
+      </c>
+      <c r="B373" t="s">
+        <v>840</v>
+      </c>
+      <c r="C373">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A374">
+        <v>2018</v>
+      </c>
+      <c r="B374" t="s">
+        <v>841</v>
+      </c>
+      <c r="C374">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A375">
+        <v>2018</v>
+      </c>
+      <c r="B375" t="s">
+        <v>4</v>
+      </c>
+      <c r="C375">
+        <v>141918</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A376">
+        <v>2018</v>
+      </c>
+      <c r="B376" t="s">
+        <v>3</v>
+      </c>
+      <c r="C376">
+        <v>27368</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A377">
+        <v>2018</v>
+      </c>
+      <c r="B377" t="s">
+        <v>837</v>
+      </c>
+      <c r="C377">
+        <v>32903</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A378">
+        <v>2018</v>
+      </c>
+      <c r="B378" t="s">
+        <v>8</v>
+      </c>
+      <c r="C378">
+        <v>8406</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A379">
+        <v>2018</v>
+      </c>
+      <c r="B379" t="s">
+        <v>7</v>
+      </c>
+      <c r="C379">
+        <v>2740</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A380">
+        <v>2018</v>
+      </c>
+      <c r="B380" t="s">
+        <v>6</v>
+      </c>
+      <c r="C380">
+        <v>20945</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A381">
+        <v>2018</v>
+      </c>
+      <c r="B381" t="s">
+        <v>833</v>
+      </c>
+      <c r="C381">
+        <v>67537</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A382">
+        <v>2018</v>
+      </c>
+      <c r="B382" t="s">
+        <v>840</v>
+      </c>
+      <c r="C382">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A383">
+        <v>2018</v>
+      </c>
+      <c r="B383" t="s">
+        <v>841</v>
+      </c>
+      <c r="C383">
+        <v>6785</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A384">
+        <v>2018</v>
+      </c>
+      <c r="B384" t="s">
+        <v>4</v>
+      </c>
+      <c r="C384">
+        <v>78141</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A385">
+        <v>2018</v>
+      </c>
+      <c r="B385" t="s">
+        <v>837</v>
+      </c>
+      <c r="C385">
+        <v>12829</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A386">
+        <v>2018</v>
+      </c>
+      <c r="B386" t="s">
+        <v>8</v>
+      </c>
+      <c r="C386">
+        <v>10449</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A387">
+        <v>2018</v>
+      </c>
+      <c r="B387" t="s">
+        <v>7</v>
+      </c>
+      <c r="C387">
+        <v>5171</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A388">
+        <v>2018</v>
+      </c>
+      <c r="B388" t="s">
+        <v>6</v>
+      </c>
+      <c r="C388">
+        <v>24453</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A389">
+        <v>2018</v>
+      </c>
+      <c r="B389" t="s">
+        <v>833</v>
+      </c>
+      <c r="C389">
+        <v>34395</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A390">
+        <v>2018</v>
+      </c>
+      <c r="B390" t="s">
+        <v>840</v>
+      </c>
+      <c r="C390">
+        <v>3264</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A391">
+        <v>2018</v>
+      </c>
+      <c r="B391" t="s">
+        <v>841</v>
+      </c>
+      <c r="C391">
+        <v>42781</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A392">
+        <v>2018</v>
+      </c>
+      <c r="B392" t="s">
+        <v>837</v>
+      </c>
+      <c r="C392">
+        <v>14565</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A393">
+        <v>2018</v>
+      </c>
+      <c r="B393" t="s">
+        <v>8</v>
+      </c>
+      <c r="C393">
+        <v>7143</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A394">
+        <v>2018</v>
+      </c>
+      <c r="B394" t="s">
+        <v>842</v>
+      </c>
+      <c r="C394">
+        <v>72109</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A395">
+        <v>2018</v>
+      </c>
+      <c r="B395" t="s">
+        <v>7</v>
+      </c>
+      <c r="C395">
+        <v>4257</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A396">
+        <v>2018</v>
+      </c>
+      <c r="B396" t="s">
+        <v>6</v>
+      </c>
+      <c r="C396">
+        <v>25150</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A397">
+        <v>2018</v>
+      </c>
+      <c r="B397" t="s">
+        <v>833</v>
+      </c>
+      <c r="C397">
+        <v>38909</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A398">
+        <v>2018</v>
+      </c>
+      <c r="B398" t="s">
+        <v>840</v>
+      </c>
+      <c r="C398">
+        <v>3331</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A399">
+        <v>2018</v>
+      </c>
+      <c r="B399" t="s">
+        <v>841</v>
+      </c>
+      <c r="C399">
+        <v>23849</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A400">
+        <v>2017</v>
+      </c>
+      <c r="B400" t="s">
+        <v>837</v>
+      </c>
+      <c r="C400">
+        <v>10792</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A401">
+        <v>2017</v>
+      </c>
+      <c r="B401" t="s">
+        <v>8</v>
+      </c>
+      <c r="C401">
+        <v>9920</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A402">
+        <v>2017</v>
+      </c>
+      <c r="B402" t="s">
+        <v>842</v>
+      </c>
+      <c r="C402">
+        <v>54577</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A403">
+        <v>2017</v>
+      </c>
+      <c r="B403" t="s">
+        <v>7</v>
+      </c>
+      <c r="C403">
+        <v>6057</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A404">
+        <v>2017</v>
+      </c>
+      <c r="B404" t="s">
+        <v>843</v>
+      </c>
+      <c r="C404">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A405">
+        <v>2017</v>
+      </c>
+      <c r="B405" t="s">
+        <v>6</v>
+      </c>
+      <c r="C405">
+        <v>17360</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A406">
+        <v>2017</v>
+      </c>
+      <c r="B406" t="s">
+        <v>833</v>
+      </c>
+      <c r="C406">
+        <v>32593</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A407">
+        <v>2017</v>
+      </c>
+      <c r="B407" t="s">
+        <v>837</v>
+      </c>
+      <c r="C407">
+        <v>5358</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A408">
+        <v>2017</v>
+      </c>
+      <c r="B408" t="s">
+        <v>8</v>
+      </c>
+      <c r="C408">
+        <v>14880</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A409">
+        <v>2017</v>
+      </c>
+      <c r="B409" t="s">
+        <v>842</v>
+      </c>
+      <c r="C409">
+        <v>48960</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A410">
+        <v>2017</v>
+      </c>
+      <c r="B410" t="s">
+        <v>7</v>
+      </c>
+      <c r="C410">
+        <v>4028</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A411">
+        <v>2017</v>
+      </c>
+      <c r="B411" t="s">
+        <v>843</v>
+      </c>
+      <c r="C411">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A412">
+        <v>2017</v>
+      </c>
+      <c r="B412" t="s">
+        <v>6</v>
+      </c>
+      <c r="C412">
+        <v>18985</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A413">
+        <v>2017</v>
+      </c>
+      <c r="B413" t="s">
+        <v>837</v>
+      </c>
+      <c r="C413">
+        <v>9131</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A414">
+        <v>2017</v>
+      </c>
+      <c r="B414" t="s">
+        <v>8</v>
+      </c>
+      <c r="C414">
+        <v>14896</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A415">
+        <v>2017</v>
+      </c>
+      <c r="B415" t="s">
+        <v>842</v>
+      </c>
+      <c r="C415">
+        <v>40801</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A416">
+        <v>2017</v>
+      </c>
+      <c r="B416" t="s">
+        <v>7</v>
+      </c>
+      <c r="C416">
+        <v>4572</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A417">
+        <v>2017</v>
+      </c>
+      <c r="B417" t="s">
+        <v>843</v>
+      </c>
+      <c r="C417">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A418">
+        <v>2017</v>
+      </c>
+      <c r="B418" t="s">
+        <v>6</v>
+      </c>
+      <c r="C418">
+        <v>20146</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A419">
+        <v>2017</v>
+      </c>
+      <c r="B419" t="s">
+        <v>837</v>
+      </c>
+      <c r="C419">
+        <v>9811</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A420">
+        <v>2017</v>
+      </c>
+      <c r="B420" t="s">
+        <v>8</v>
+      </c>
+      <c r="C420">
+        <v>13436</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A421">
+        <v>2017</v>
+      </c>
+      <c r="B421" t="s">
+        <v>842</v>
+      </c>
+      <c r="C421">
+        <v>66198</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A422">
+        <v>2017</v>
+      </c>
+      <c r="B422" t="s">
+        <v>7</v>
+      </c>
+      <c r="C422">
+        <v>10315</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A423">
+        <v>2017</v>
+      </c>
+      <c r="B423" t="s">
+        <v>843</v>
+      </c>
+      <c r="C423">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A424">
+        <v>2017</v>
+      </c>
+      <c r="B424" t="s">
+        <v>6</v>
+      </c>
+      <c r="C424">
+        <v>18237</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A425">
+        <v>2016</v>
+      </c>
+      <c r="B425" t="s">
+        <v>837</v>
+      </c>
+      <c r="C425">
+        <v>12754</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A426">
+        <v>2016</v>
+      </c>
+      <c r="B426" t="s">
+        <v>8</v>
+      </c>
+      <c r="C426">
+        <v>13277</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A427">
+        <v>2016</v>
+      </c>
+      <c r="B427" t="s">
+        <v>842</v>
+      </c>
+      <c r="C427">
+        <v>77398</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A428">
+        <v>2016</v>
+      </c>
+      <c r="B428" t="s">
+        <v>7</v>
+      </c>
+      <c r="C428">
+        <v>17602</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A429">
+        <v>2016</v>
+      </c>
+      <c r="B429" t="s">
+        <v>843</v>
+      </c>
+      <c r="C429">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="430" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A430">
+        <v>2016</v>
+      </c>
+      <c r="B430" t="s">
+        <v>844</v>
+      </c>
+      <c r="C430">
+        <v>7966</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A431">
+        <v>2016</v>
+      </c>
+      <c r="B431" t="s">
+        <v>837</v>
+      </c>
+      <c r="C431">
+        <v>9207</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A432">
+        <v>2016</v>
+      </c>
+      <c r="B432" t="s">
+        <v>8</v>
+      </c>
+      <c r="C432">
+        <v>9566</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A433">
+        <v>2016</v>
+      </c>
+      <c r="B433" t="s">
+        <v>842</v>
+      </c>
+      <c r="C433">
+        <v>63754</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A434">
+        <v>2016</v>
+      </c>
+      <c r="B434" t="s">
+        <v>7</v>
+      </c>
+      <c r="C434">
+        <v>10573</v>
+      </c>
+    </row>
+    <row r="435" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A435">
+        <v>2016</v>
+      </c>
+      <c r="B435" t="s">
+        <v>843</v>
+      </c>
+      <c r="C435">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A436">
+        <v>2016</v>
+      </c>
+      <c r="B436" t="s">
+        <v>844</v>
+      </c>
+      <c r="C436">
+        <v>4769</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A437">
+        <v>2016</v>
+      </c>
+      <c r="B437" t="s">
+        <v>837</v>
+      </c>
+      <c r="C437">
+        <v>32073</v>
+      </c>
+    </row>
+    <row r="438" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A438">
+        <v>2016</v>
+      </c>
+      <c r="B438" t="s">
+        <v>8</v>
+      </c>
+      <c r="C438">
+        <v>18669</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A439">
+        <v>2016</v>
+      </c>
+      <c r="B439" t="s">
+        <v>842</v>
+      </c>
+      <c r="C439">
+        <v>63475</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A440">
+        <v>2016</v>
+      </c>
+      <c r="B440" t="s">
+        <v>7</v>
+      </c>
+      <c r="C440">
+        <v>14403</v>
+      </c>
+    </row>
+    <row r="441" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A441">
+        <v>2016</v>
+      </c>
+      <c r="B441" t="s">
+        <v>843</v>
+      </c>
+      <c r="C441">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A442">
+        <v>2016</v>
+      </c>
+      <c r="B442" t="s">
+        <v>844</v>
+      </c>
+      <c r="C442">
+        <v>4085</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A443">
+        <v>2016</v>
+      </c>
+      <c r="B443" t="s">
+        <v>837</v>
+      </c>
+      <c r="C443">
+        <v>18716</v>
+      </c>
+    </row>
+    <row r="444" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A444">
+        <v>2016</v>
+      </c>
+      <c r="B444" t="s">
+        <v>8</v>
+      </c>
+      <c r="C444">
+        <v>18109</v>
+      </c>
+    </row>
+    <row r="445" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A445">
+        <v>2016</v>
+      </c>
+      <c r="B445" t="s">
+        <v>842</v>
+      </c>
+      <c r="C445">
+        <v>58834</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A446">
+        <v>2016</v>
+      </c>
+      <c r="B446" t="s">
+        <v>7</v>
+      </c>
+      <c r="C446">
+        <v>22661</v>
+      </c>
+    </row>
+    <row r="447" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A447">
+        <v>2016</v>
+      </c>
+      <c r="B447" t="s">
+        <v>843</v>
+      </c>
+      <c r="C447">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A448">
+        <v>2016</v>
+      </c>
+      <c r="B448" t="s">
+        <v>844</v>
+      </c>
+      <c r="C448">
+        <v>4618</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A449">
+        <v>2015</v>
+      </c>
+      <c r="B449" t="s">
+        <v>845</v>
+      </c>
+      <c r="C449">
+        <v>34432</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A450">
+        <v>2015</v>
+      </c>
+      <c r="B450" t="s">
+        <v>845</v>
+      </c>
+      <c r="C450">
+        <v>10302</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A451">
+        <v>2015</v>
+      </c>
+      <c r="B451" t="s">
+        <v>846</v>
+      </c>
+      <c r="C451">
+        <v>17056</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A452">
+        <v>2015</v>
+      </c>
+      <c r="B452" t="s">
+        <v>847</v>
+      </c>
+      <c r="C452">
+        <v>27172</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A453">
+        <v>2015</v>
+      </c>
+      <c r="B453" t="s">
+        <v>848</v>
+      </c>
+      <c r="C453">
+        <v>62881</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A454">
+        <v>2015</v>
+      </c>
+      <c r="B454" t="s">
+        <v>849</v>
+      </c>
+      <c r="C454">
+        <v>23118</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A455">
+        <v>2015</v>
+      </c>
+      <c r="B455" t="s">
+        <v>850</v>
+      </c>
+      <c r="C455">
+        <v>3847</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A456">
+        <v>2015</v>
+      </c>
+      <c r="B456" t="s">
+        <v>845</v>
+      </c>
+      <c r="C456">
+        <v>59506</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A457">
+        <v>2015</v>
+      </c>
+      <c r="B457" t="s">
+        <v>845</v>
+      </c>
+      <c r="C457">
+        <v>13236</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A458">
+        <v>2015</v>
+      </c>
+      <c r="B458" t="s">
+        <v>837</v>
+      </c>
+      <c r="C458">
+        <v>22640</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A459">
+        <v>2015</v>
+      </c>
+      <c r="B459" t="s">
+        <v>8</v>
+      </c>
+      <c r="C459">
+        <v>40643</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A460">
+        <v>2015</v>
+      </c>
+      <c r="B460" t="s">
+        <v>851</v>
+      </c>
+      <c r="C460">
+        <v>90274</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A461">
+        <v>2015</v>
+      </c>
+      <c r="B461" t="s">
+        <v>849</v>
+      </c>
+      <c r="C461">
+        <v>34892</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A462">
+        <v>2015</v>
+      </c>
+      <c r="B462" t="s">
+        <v>26</v>
+      </c>
+      <c r="C462">
+        <v>83703</v>
+      </c>
+    </row>
+    <row r="463" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A463">
+        <v>2015</v>
+      </c>
+      <c r="B463" t="s">
+        <v>26</v>
+      </c>
+      <c r="C463">
+        <v>11830</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A464">
+        <v>2015</v>
+      </c>
+      <c r="B464" t="s">
+        <v>837</v>
+      </c>
+      <c r="C464">
+        <v>22112</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A465">
+        <v>2015</v>
+      </c>
+      <c r="B465" t="s">
+        <v>8</v>
+      </c>
+      <c r="C465">
+        <v>108570</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A466">
+        <v>2015</v>
+      </c>
+      <c r="B466" t="s">
+        <v>842</v>
+      </c>
+      <c r="C466">
+        <v>76421</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A467">
+        <v>2015</v>
+      </c>
+      <c r="B467" t="s">
+        <v>26</v>
+      </c>
+      <c r="C467">
+        <v>106222</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A468">
+        <v>2015</v>
+      </c>
+      <c r="B468" t="s">
+        <v>26</v>
+      </c>
+      <c r="C468">
+        <v>11408</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A469">
+        <v>2015</v>
+      </c>
+      <c r="B469" t="s">
+        <v>837</v>
+      </c>
+      <c r="C469">
+        <v>21961</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A470">
+        <v>2015</v>
+      </c>
+      <c r="B470" t="s">
+        <v>8</v>
+      </c>
+      <c r="C470">
+        <v>60813</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A471">
+        <v>2014</v>
+      </c>
+      <c r="B471" t="s">
+        <v>26</v>
+      </c>
+      <c r="C471">
+        <v>118910</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A472">
+        <v>2014</v>
+      </c>
+      <c r="B472" t="s">
+        <v>26</v>
+      </c>
+      <c r="C472">
+        <v>9897</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A473">
+        <v>2014</v>
+      </c>
+      <c r="B473" t="s">
+        <v>837</v>
+      </c>
+      <c r="C473">
+        <v>32903</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A474">
+        <v>2014</v>
+      </c>
+      <c r="B474" t="s">
+        <v>8</v>
+      </c>
+      <c r="C474">
+        <v>38707</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A475">
+        <v>2014</v>
+      </c>
+      <c r="B475" t="s">
+        <v>26</v>
+      </c>
+      <c r="C475">
+        <v>129234</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A476">
+        <v>2014</v>
+      </c>
+      <c r="B476" t="s">
+        <v>26</v>
+      </c>
+      <c r="C476">
+        <v>10757</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A477">
+        <v>2014</v>
+      </c>
+      <c r="B477" t="s">
+        <v>837</v>
+      </c>
+      <c r="C477">
+        <v>38035</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A478">
+        <v>2022</v>
+      </c>
+      <c r="B478" t="s">
+        <v>829</v>
+      </c>
+      <c r="C478">
+        <v>229</v>
+      </c>
+      <c r="D478">
+        <v>510142</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A479">
+        <v>2022</v>
+      </c>
+      <c r="B479" t="s">
+        <v>23</v>
+      </c>
+      <c r="C479">
+        <v>532</v>
+      </c>
+      <c r="D479">
+        <v>311490</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A480">
+        <v>2022</v>
+      </c>
+      <c r="B480" t="s">
+        <v>830</v>
+      </c>
+      <c r="C480">
+        <v>21098</v>
+      </c>
+      <c r="D480">
+        <v>907032</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A481">
+        <v>2022</v>
+      </c>
+      <c r="B481" t="s">
+        <v>831</v>
+      </c>
+      <c r="C481">
+        <v>10420</v>
+      </c>
+      <c r="D481">
+        <v>1488596</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A482">
+        <v>2022</v>
+      </c>
+      <c r="B482" t="s">
+        <v>829</v>
+      </c>
+      <c r="C482">
+        <v>203</v>
+      </c>
+      <c r="D482">
+        <v>510142</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A483">
+        <v>2022</v>
+      </c>
+      <c r="B483" t="s">
+        <v>23</v>
+      </c>
+      <c r="C483">
+        <v>300</v>
+      </c>
+      <c r="D483">
+        <v>311490</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A484">
+        <v>2022</v>
+      </c>
+      <c r="B484" t="s">
+        <v>830</v>
+      </c>
+      <c r="C484">
+        <v>15220</v>
+      </c>
+      <c r="D484">
+        <v>907032</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A485">
+        <v>2022</v>
+      </c>
+      <c r="B485" t="s">
+        <v>831</v>
+      </c>
+      <c r="C485">
+        <v>10152</v>
+      </c>
+      <c r="D485">
+        <v>1488596</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A486">
+        <v>2022</v>
+      </c>
+      <c r="B486" t="s">
+        <v>832</v>
+      </c>
+      <c r="C486">
+        <v>17933</v>
+      </c>
+      <c r="D486">
+        <v>994079</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A487">
+        <v>2022</v>
+      </c>
+      <c r="B487" t="s">
+        <v>829</v>
+      </c>
+      <c r="C487">
+        <v>319</v>
+      </c>
+      <c r="D487">
+        <v>510142</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A488">
+        <v>2022</v>
+      </c>
+      <c r="B488" t="s">
+        <v>23</v>
+      </c>
+      <c r="C488">
+        <v>545</v>
+      </c>
+      <c r="D488">
+        <v>311490</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A489">
+        <v>2022</v>
+      </c>
+      <c r="B489" t="s">
+        <v>830</v>
+      </c>
+      <c r="C489">
+        <v>40248</v>
+      </c>
+      <c r="D489">
+        <v>917218</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A490">
+        <v>2022</v>
+      </c>
+      <c r="B490" t="s">
+        <v>831</v>
+      </c>
+      <c r="C490">
+        <v>20989</v>
+      </c>
+      <c r="D490">
+        <v>1488596</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A491">
+        <v>2022</v>
+      </c>
+      <c r="B491" t="s">
+        <v>832</v>
+      </c>
+      <c r="C491">
+        <v>20694</v>
+      </c>
+      <c r="D491">
+        <v>1290978</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A492">
+        <v>2022</v>
+      </c>
+      <c r="B492" t="s">
+        <v>829</v>
+      </c>
+      <c r="C492">
+        <v>566</v>
+      </c>
+      <c r="D492">
+        <v>510142</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A493">
+        <v>2022</v>
+      </c>
+      <c r="B493" t="s">
+        <v>23</v>
+      </c>
+      <c r="C493">
+        <v>713</v>
+      </c>
+      <c r="D493">
+        <v>311490</v>
+      </c>
+    </row>
+    <row r="494" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A494">
+        <v>2022</v>
+      </c>
+      <c r="B494" t="s">
+        <v>3</v>
+      </c>
+      <c r="C494">
+        <v>27149</v>
+      </c>
+      <c r="D494">
+        <v>1824542</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A495">
+        <v>2022</v>
+      </c>
+      <c r="B495" t="s">
+        <v>830</v>
+      </c>
+      <c r="C495">
+        <v>55888</v>
+      </c>
+      <c r="D495">
+        <v>918154</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A496">
+        <v>2022</v>
+      </c>
+      <c r="B496" t="s">
+        <v>831</v>
+      </c>
+      <c r="C496">
+        <v>22909</v>
+      </c>
+      <c r="D496">
+        <v>1581031</v>
+      </c>
+    </row>
+    <row r="497" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A497">
+        <v>2022</v>
+      </c>
+      <c r="B497" t="s">
+        <v>832</v>
+      </c>
+      <c r="C497">
+        <v>47480</v>
+      </c>
+      <c r="D497">
+        <v>1941118</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A498">
+        <v>2021</v>
+      </c>
+      <c r="B498" t="s">
+        <v>829</v>
+      </c>
+      <c r="C498">
+        <v>944</v>
+      </c>
+      <c r="D498">
+        <v>510142</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A499">
+        <v>2021</v>
+      </c>
+      <c r="B499" t="s">
+        <v>833</v>
+      </c>
+      <c r="C499">
+        <v>15289</v>
+      </c>
+      <c r="D499">
+        <v>449951</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A500">
+        <v>2021</v>
+      </c>
+      <c r="B500" t="s">
+        <v>23</v>
+      </c>
+      <c r="C500">
+        <v>1648</v>
+      </c>
+      <c r="D500">
+        <v>311490</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A501">
+        <v>2021</v>
+      </c>
+      <c r="B501" t="s">
+        <v>3</v>
+      </c>
+      <c r="C501">
+        <v>34466</v>
+      </c>
+      <c r="D501">
+        <v>1824542</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A502">
+        <v>2021</v>
+      </c>
+      <c r="B502" t="s">
+        <v>830</v>
+      </c>
+      <c r="C502">
+        <v>59742</v>
+      </c>
+      <c r="D502">
+        <v>1436456</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A503">
+        <v>2021</v>
+      </c>
+      <c r="B503" t="s">
+        <v>834</v>
+      </c>
+      <c r="C503">
+        <v>42859</v>
+      </c>
+      <c r="D503">
+        <v>1694017</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A504">
+        <v>2021</v>
+      </c>
+      <c r="B504" t="s">
+        <v>832</v>
+      </c>
+      <c r="C504">
+        <v>45209</v>
+      </c>
+      <c r="D504">
+        <v>1941118</v>
+      </c>
+    </row>
+    <row r="505" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A505">
+        <v>2021</v>
+      </c>
+      <c r="B505" t="s">
+        <v>835</v>
+      </c>
+      <c r="C505">
+        <v>4203</v>
+      </c>
+      <c r="D505">
+        <v>14541</v>
+      </c>
+    </row>
+    <row r="506" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A506">
+        <v>2021</v>
+      </c>
+      <c r="B506" t="s">
+        <v>829</v>
+      </c>
+      <c r="C506">
+        <v>1618</v>
+      </c>
+      <c r="D506">
+        <v>510142</v>
+      </c>
+    </row>
+    <row r="507" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A507">
+        <v>2021</v>
+      </c>
+      <c r="B507" t="s">
+        <v>833</v>
+      </c>
+      <c r="C507">
+        <v>16473</v>
+      </c>
+      <c r="D507">
+        <v>449951</v>
+      </c>
+    </row>
+    <row r="508" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A508">
+        <v>2021</v>
+      </c>
+      <c r="B508" t="s">
+        <v>23</v>
+      </c>
+      <c r="C508">
+        <v>2025</v>
+      </c>
+      <c r="D508">
+        <v>311490</v>
+      </c>
+    </row>
+    <row r="509" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A509">
+        <v>2021</v>
+      </c>
+      <c r="B509" t="s">
+        <v>3</v>
+      </c>
+      <c r="C509">
+        <v>33918</v>
+      </c>
+      <c r="D509">
+        <v>1824542</v>
+      </c>
+    </row>
+    <row r="510" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A510">
+        <v>2021</v>
+      </c>
+      <c r="B510" t="s">
+        <v>830</v>
+      </c>
+      <c r="C510">
+        <v>58147</v>
+      </c>
+      <c r="D510">
+        <v>1915274</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A511">
+        <v>2021</v>
+      </c>
+      <c r="B511" t="s">
+        <v>834</v>
+      </c>
+      <c r="C511">
+        <v>37574</v>
+      </c>
+      <c r="D511">
+        <v>1694017</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A512">
+        <v>2021</v>
+      </c>
+      <c r="B512" t="s">
+        <v>836</v>
+      </c>
+      <c r="C512">
+        <v>79809</v>
+      </c>
+      <c r="D512">
+        <v>2911677</v>
+      </c>
+    </row>
+    <row r="513" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A513">
+        <v>2021</v>
+      </c>
+      <c r="B513" t="s">
+        <v>829</v>
+      </c>
+      <c r="C513">
+        <v>1658</v>
+      </c>
+      <c r="D513">
+        <v>510142</v>
+      </c>
+    </row>
+    <row r="514" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A514">
+        <v>2021</v>
+      </c>
+      <c r="B514" t="s">
+        <v>833</v>
+      </c>
+      <c r="C514">
+        <v>20176</v>
+      </c>
+      <c r="D514">
+        <v>449951</v>
+      </c>
+    </row>
+    <row r="515" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A515">
+        <v>2021</v>
+      </c>
+      <c r="B515" t="s">
+        <v>23</v>
+      </c>
+      <c r="C515">
+        <v>2682</v>
+      </c>
+      <c r="D515">
+        <v>311490</v>
+      </c>
+    </row>
+    <row r="516" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A516">
+        <v>2021</v>
+      </c>
+      <c r="B516" t="s">
+        <v>4</v>
+      </c>
+      <c r="C516">
+        <v>3491</v>
+      </c>
+      <c r="D516">
+        <v>275034</v>
+      </c>
+    </row>
+    <row r="517" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A517">
+        <v>2021</v>
+      </c>
+      <c r="B517" t="s">
+        <v>3</v>
+      </c>
+      <c r="C517">
+        <v>41527</v>
+      </c>
+      <c r="D517">
+        <v>1824542</v>
+      </c>
+    </row>
+    <row r="518" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A518">
+        <v>2021</v>
+      </c>
+      <c r="B518" t="s">
+        <v>830</v>
+      </c>
+      <c r="C518">
+        <v>57209</v>
+      </c>
+      <c r="D518">
+        <v>1915274</v>
+      </c>
+    </row>
+    <row r="519" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A519">
+        <v>2021</v>
+      </c>
+      <c r="B519" t="s">
+        <v>834</v>
+      </c>
+      <c r="C519">
+        <v>33186</v>
+      </c>
+      <c r="D519">
+        <v>1694017</v>
+      </c>
+    </row>
+    <row r="520" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A520">
+        <v>2021</v>
+      </c>
+      <c r="B520" t="s">
+        <v>836</v>
+      </c>
+      <c r="C520">
+        <v>107033</v>
+      </c>
+      <c r="D520">
+        <v>2911677</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Worked on SEC Scraper
</commit_message>
<xml_diff>
--- a/Master.xlsx
+++ b/Master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasg17/Documents/GitHub/Health-Innovation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD652C06-51BB-E048-8806-824B41081D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{457C242F-85BA-1B4E-96EC-7A7AFC6B6F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="760" windowWidth="28060" windowHeight="17440" xr2:uid="{7B871D28-6C56-6A4C-8DC7-F3E0A8269B8A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4827" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4839" uniqueCount="457">
   <si>
     <t>Year</t>
   </si>
@@ -1762,7 +1762,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF57BEF-A7F1-EB4D-BEC9-B2B3C82B4989}">
   <dimension ref="A1:E239"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="G239" sqref="G239"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -42023,7 +42025,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF1BB6E-2638-6F4C-AE3A-D3BA1AF8B8FD}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -42745,6 +42747,108 @@
         <v>7158647</v>
       </c>
     </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2024</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>230736820</v>
+      </c>
+      <c r="E43">
+        <v>6727021</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2024</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44">
+        <v>189311347</v>
+      </c>
+      <c r="E44">
+        <v>2788912</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2023</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45">
+        <v>521901338</v>
+      </c>
+      <c r="E45">
+        <v>13727021</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2023</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>172075870</v>
+      </c>
+      <c r="E46">
+        <v>2788912</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2023</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>543306741</v>
+      </c>
+      <c r="E47">
+        <v>16208435</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2023</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48">
+        <v>168924400</v>
+      </c>
+      <c r="E48">
+        <v>2788912</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>